<commit_message>
add participants from 28th to 34th B2GM, add city pairs and CO2 between airports
</commit_message>
<xml_diff>
--- a/GIT/BelleII/Climate/CDATA/Airfares_CityPairs_20190929.xlsx
+++ b/GIT/BelleII/Climate/CDATA/Airfares_CityPairs_20190929.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djaffe/PythonScripts/CDATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djaffe/work/GIT/BelleII/Climate/CDATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EA004BD-4EA9-C74F-8969-C84823666C8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DA6D7-0911-4B47-9E23-4037DA8A0FBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="21540" windowHeight="16540" xr2:uid="{589D98D2-F20B-7441-8F47-590390F67DE1}"/>
+    <workbookView xWindow="3200" yWindow="960" windowWidth="21540" windowHeight="16540" xr2:uid="{589D98D2-F20B-7441-8F47-590390F67DE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Airfares_CityPairs_20190929" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
   <si>
     <t>Origin</t>
   </si>
@@ -244,6 +244,42 @@
   </si>
   <si>
     <t>S7 Airlines, one stop</t>
+  </si>
+  <si>
+    <t>Kiev</t>
+  </si>
+  <si>
+    <t>Ljubliana</t>
+  </si>
+  <si>
+    <t>Alternate origin name</t>
+  </si>
+  <si>
+    <t>Bombay</t>
+  </si>
+  <si>
+    <t>Turin</t>
+  </si>
+  <si>
+    <t>Madras</t>
+  </si>
+  <si>
+    <t>PITTSBURGH (PENNSYLVA)</t>
+  </si>
+  <si>
+    <t>Tel-Aviv</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Napoli</t>
+  </si>
+  <si>
+    <t>Muenchen</t>
+  </si>
+  <si>
+    <t>Orsay</t>
   </si>
 </sst>
 </file>
@@ -292,10 +328,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993C0FB7-B57B-7B4D-B10D-AF922B300B9C}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -621,10 +660,11 @@
     <col min="1" max="1" width="22.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="36.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,11 +674,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -648,11 +691,11 @@
       <c r="C2" s="1">
         <v>1333</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -662,11 +705,11 @@
       <c r="C3" s="1">
         <v>1093</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -676,11 +719,11 @@
       <c r="C4" s="1">
         <v>2076</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -690,11 +733,11 @@
       <c r="C5" s="1">
         <v>1364</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -705,10 +748,13 @@
         <v>724</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -718,11 +764,11 @@
       <c r="C7" s="1">
         <v>1770</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -732,11 +778,11 @@
       <c r="C8" s="1">
         <v>1614</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -746,11 +792,11 @@
       <c r="C9" s="1">
         <v>1591</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -760,11 +806,11 @@
       <c r="C10" s="1">
         <v>1791</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -774,11 +820,11 @@
       <c r="C11" s="1">
         <v>1051</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -789,10 +835,13 @@
         <v>1400</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -802,11 +851,11 @@
       <c r="C13" s="1">
         <v>1600</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -817,10 +866,13 @@
         <v>1655</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -831,10 +883,13 @@
         <v>1559</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -844,11 +899,11 @@
       <c r="C16" s="1">
         <v>1538</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -858,11 +913,11 @@
       <c r="C17" s="1">
         <v>787</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -873,10 +928,13 @@
         <v>1325</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -886,11 +944,11 @@
       <c r="C19" s="1">
         <v>1514</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -900,11 +958,11 @@
       <c r="C20" s="1">
         <v>1286</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -914,11 +972,11 @@
       <c r="C21" s="1">
         <v>547</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -928,11 +986,11 @@
       <c r="C22" s="1">
         <v>246</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -942,11 +1000,11 @@
       <c r="C23" s="1">
         <v>837</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -956,11 +1014,11 @@
       <c r="C24" s="1">
         <v>1087</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -971,10 +1029,13 @@
         <v>636</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -984,11 +1045,11 @@
       <c r="C26" s="1">
         <v>196</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -998,11 +1059,11 @@
       <c r="C27" s="1">
         <v>441</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -1012,11 +1073,11 @@
       <c r="C28" s="1">
         <v>1151</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
@@ -1026,11 +1087,11 @@
       <c r="C29" s="1">
         <v>615</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
@@ -1040,11 +1101,11 @@
       <c r="C30" s="1">
         <v>1080</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
@@ -1054,11 +1115,11 @@
       <c r="C31" s="1">
         <v>1172</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
@@ -1068,11 +1129,11 @@
       <c r="C32" s="1">
         <v>489</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
@@ -1083,10 +1144,13 @@
         <v>785</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
@@ -1097,10 +1161,13 @@
         <v>1410</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
@@ -1110,11 +1177,11 @@
       <c r="C35" s="1">
         <v>784</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
@@ -1124,11 +1191,11 @@
       <c r="C36" s="1">
         <v>698</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>60</v>
       </c>
@@ -1138,11 +1205,11 @@
       <c r="C37" s="1">
         <v>1533</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1152,11 +1219,11 @@
       <c r="C38" s="1">
         <v>278</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>64</v>
       </c>
@@ -1166,11 +1233,11 @@
       <c r="C39" s="1">
         <v>1033</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -1181,10 +1248,13 @@
         <v>1285</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -1195,10 +1265,13 @@
         <v>1255</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>68</v>
       </c>
@@ -1209,10 +1282,13 @@
         <v>1197</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
@@ -1222,11 +1298,11 @@
       <c r="C43" s="1">
         <v>1115</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
@@ -1236,7 +1312,7 @@
       <c r="C44" s="1">
         <v>1017</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>